<commit_message>
Added Linear Sine Model
</commit_message>
<xml_diff>
--- a/Datasets/Predictions.xlsx
+++ b/Datasets/Predictions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1080" yWindow="820" windowWidth="28040" windowHeight="17440" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1080" yWindow="820" windowWidth="28040" windowHeight="17440" tabRatio="600" firstSheet="0" activeTab="9" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02-19-2024" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,22 +13,32 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02-23-2024" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02-24-2024" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02-25-2024" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02-26-2024" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02-27-2024" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02-28-2024" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02-29-2024" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0009999999999999445"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="12"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -72,12 +82,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -165,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -183,6 +208,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -916,6 +944,952 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Linear Predicted Difference</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>XGBoost Predicted Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>pollster_CBS News</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2.547517477703314</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.428045749664307</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>pollster_CNN</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3.542599656047323</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2.704452753067017</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Daily Kos/Civiqs</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1475346496806464</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.6290268301963806</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Data for Progress (D)**</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-1.695095057326953</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-2.005419492721558</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Economist/YouGov</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4836790922487668</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.002308783587068319</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Emerson</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2.256514165598384</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.6656510233879089</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>pollster_FOX News</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.886527903179886</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2.818512916564941</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Federalist/Susquehanna</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-1.632845579626932</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-2.209126472473145</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Grinnell/Selzer</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.6688237452186248</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1.1358642578125</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>pollster_HarrisX**</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>6.049178216559968</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2.914090871810913</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Harvard-Harris</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>5.41086223468176</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4.099342823028564</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>pollster_I&amp;I/TIPP</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1.035718998723315</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8425951600074768</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Insider Advantage</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5.53436035667767</v>
+      </c>
+      <c r="C14" t="n">
+        <v>4.250433444976807</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>pollster_InsiderAdvantage</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.198330675154928</v>
+      </c>
+      <c r="C15" t="n">
+        <v>7.006680965423584</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Marist</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-0.02135349045243551</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.9264268279075623</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Marquette</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>3.09105386168518</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.376412630081177</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Morning Consult</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.7764275275003487</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1.009001135826111</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>pollster_NBC News</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1.431118299358459</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3.303689002990723</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>pollster_NPR/PBS/Marist</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-1.249611646500263</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-1.770082592964172</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>pollster_NY Times/Siena</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-0.5747895261200542</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-2.049990892410278</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="inlineStr">
+        <is>
+          <t>pollster_New York Post</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>3.843406414006734</v>
+      </c>
+      <c r="C22" t="n">
+        <v>3.715561151504517</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>pollster_PPP (D)</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>-2.116474305745018</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-1.068375587463379</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Politico/Morning Consult</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.7507445095424088</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.6613050103187561</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Quinnipiac</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-1.416939400300456</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-5.379960536956787</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Rasmussen Reports</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>6.067177206265816</v>
+      </c>
+      <c r="C26" t="n">
+        <v>5.243505954742432</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Reuters/Ipsos</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2.507344535026708</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1.322910666465759</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>pollster_SurveyUSA</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.7327554267466669</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1.041263937950134</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Susquehanna</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>-11.19024163058532</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-7.766969203948975</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>pollster_The Messenger/HarrisX</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>3.988287976109706</v>
+      </c>
+      <c r="C30" t="n">
+        <v>3.695779085159302</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Trafalgar Group (R)</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>6.131098980884162</v>
+      </c>
+      <c r="C31" t="n">
+        <v>5.420891284942627</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="inlineStr">
+        <is>
+          <t>pollster_USA Today/Suffolk</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>-0.690513676436626</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.6375436782836914</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Wall Street Journal</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-0.1123331910887684</v>
+      </c>
+      <c r="C33" t="n">
+        <v>-2.372321844100952</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-0.7715476672023414</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.3949662446975708</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News**</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>-1.693719721348795</v>
+      </c>
+      <c r="C35" t="n">
+        <v>-3.230232238769531</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Linear Predicted Difference</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>XGBoost Predicted Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>pollster_CBS News</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2.552435299359332</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.428045749664307</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>pollster_CNN</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3.547517477703341</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2.704452753067017</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Daily Kos/Civiqs</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1524524713366651</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.6290268301963806</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Data for Progress (D)**</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-1.690177235670935</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-2.005419492721558</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Economist/YouGov</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4885969139047845</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.002308783587068319</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Emerson</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2.261431987254401</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.6656510233879089</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>pollster_FOX News</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.891445724835904</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2.818512916564941</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Federalist/Susquehanna</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-1.627927757970913</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-2.209126472473145</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Grinnell/Selzer</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.6737415668746425</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1.1358642578125</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>pollster_HarrisX**</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>6.054096038215985</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2.914090871810913</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Harvard-Harris</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>5.415780056337778</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4.099342823028564</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>pollster_I&amp;I/TIPP</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1.040636820379333</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8425951600074768</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Insider Advantage</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5.539278178333689</v>
+      </c>
+      <c r="C14" t="n">
+        <v>4.250433444976807</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>pollster_InsiderAdvantage</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.203248496810946</v>
+      </c>
+      <c r="C15" t="n">
+        <v>7.006680965423584</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Marist</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-0.01643566879641689</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.9264268279075623</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Marquette</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>3.095971683341198</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.376412630081177</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Morning Consult</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.7813453491563664</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1.009001135826111</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="inlineStr">
+        <is>
+          <t>pollster_NBC News</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1.436036121014477</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3.303689002990723</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>pollster_NPR/PBS/Marist</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-1.244693824844244</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-1.770082592964172</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="inlineStr">
+        <is>
+          <t>pollster_NY Times/Siena</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-0.5698717044640356</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-2.049990892410278</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="inlineStr">
+        <is>
+          <t>pollster_New York Post</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>3.848324235662751</v>
+      </c>
+      <c r="C22" t="n">
+        <v>3.715561151504517</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>pollster_PPP (D)</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>-2.111556484088999</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-1.068375587463379</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Politico/Morning Consult</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.7556623311984265</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.6613050103187561</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Quinnipiac</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-1.412021578644437</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-5.379960536956787</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Rasmussen Reports</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>6.072095027921835</v>
+      </c>
+      <c r="C26" t="n">
+        <v>5.243505954742432</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Reuters/Ipsos</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2.512262356682726</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1.322910666465759</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="7" t="inlineStr">
+        <is>
+          <t>pollster_SurveyUSA</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.7376732484026847</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1.041263937950134</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Susquehanna</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>-11.18532380892931</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-7.766969203948975</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="7" t="inlineStr">
+        <is>
+          <t>pollster_The Messenger/HarrisX</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>3.993205797765723</v>
+      </c>
+      <c r="C30" t="n">
+        <v>3.695779085159302</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Trafalgar Group (R)</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>6.13601680254018</v>
+      </c>
+      <c r="C31" t="n">
+        <v>5.420891284942627</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="7" t="inlineStr">
+        <is>
+          <t>pollster_USA Today/Suffolk</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>-0.6855958547806074</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.6375436782836914</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Wall Street Journal</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-0.1074153694327498</v>
+      </c>
+      <c r="C33" t="n">
+        <v>-2.372321844100952</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-0.7666298455463227</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.3949662446975708</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News**</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>-1.688801899692776</v>
+      </c>
+      <c r="C35" t="n">
+        <v>-3.230232238769531</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -2365,8 +3339,8 @@
   </sheetPr>
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -2831,10 +3805,15 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col width="29" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="23.83203125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="26" bestFit="1" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="inlineStr">
@@ -3288,6 +4267,962 @@
       </c>
       <c r="C35" t="n">
         <v>-1.243046998977661</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col width="14.33203125" customWidth="1" min="1" max="1"/>
+    <col width="21.33203125" customWidth="1" min="2" max="2"/>
+    <col width="30.1640625" customWidth="1" min="3" max="3"/>
+    <col width="26" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Linear Predicted Difference</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>XGBoost Predicted Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>pollster_CBS News</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2.540171454882834</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3.488237380981445</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>pollster_CNN</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3.535230862307769</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4.740685939788818</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Daily Kos/Civiqs</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1383365921042419</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.246809959411621</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Data for Progress (D)**</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-1.703564445490989</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.1320209056138992</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Economist/YouGov</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4932944811496229</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.004540920257568</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Emerson</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2.251293428563343</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2.620875597000122</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>pollster_FOX News</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.879825538340336</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4.764554977416992</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Federalist/Susquehanna</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-1.636396449259126</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.4275822937488556</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Grinnell/Selzer</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.6620394050698506</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2.953945159912109</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>pollster_HarrisX**</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>6.039524740601212</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4.00484561920166</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Harvard-Harris</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>5.40591095352308</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5.999284267425537</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>pollster_I&amp;I/TIPP</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1.02785531700784</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2.863374471664429</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Insider Advantage</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5.531583698295769</v>
+      </c>
+      <c r="C14" t="n">
+        <v>5.381294727325439</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>pollster_InsiderAdvantage</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.191682960520722</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8.556325912475586</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Marist</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-0.02670326269578815</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2.879482746124268</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Marquette</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>3.08622456759336</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3.559096813201904</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Morning Consult</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.7617813774915785</v>
+      </c>
+      <c r="C18" t="n">
+        <v>3.781769037246704</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>pollster_NBC News</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1.424390886507719</v>
+      </c>
+      <c r="C19" t="n">
+        <v>5.289239883422852</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>pollster_NPR/PBS/Marist</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-1.257175890628916</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.3971515595912933</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>pollster_NY Times/Siena</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-0.5808497510404571</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-0.2710374891757965</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="inlineStr">
+        <is>
+          <t>pollster_New York Post</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>3.837430441487587</v>
+      </c>
+      <c r="C22" t="n">
+        <v>5.397716045379639</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>pollster_PPP (D)</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>-2.117634228868696</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1.512863159179688</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Politico/Morning Consult</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.7489697716024137</v>
+      </c>
+      <c r="C24" t="n">
+        <v>2.562484741210938</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Quinnipiac</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-1.422339969209628</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-4.010499000549316</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Rasmussen Reports</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>6.0611688289768</v>
+      </c>
+      <c r="C26" t="n">
+        <v>6.719390392303467</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Reuters/Ipsos</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2.5009700714225</v>
+      </c>
+      <c r="C27" t="n">
+        <v>3.344177007675171</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>pollster_SurveyUSA</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.7262671085468124</v>
+      </c>
+      <c r="C28" t="n">
+        <v>2.986067771911621</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Susquehanna</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>-11.19174311749598</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-6.31898021697998</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>pollster_The Messenger/HarrisX</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>3.981825275193806</v>
+      </c>
+      <c r="C30" t="n">
+        <v>5.491835117340088</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Trafalgar Group (R)</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>6.126455107133733</v>
+      </c>
+      <c r="C31" t="n">
+        <v>6.612038135528564</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="inlineStr">
+        <is>
+          <t>pollster_USA Today/Suffolk</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>-0.6980357943649116</v>
+      </c>
+      <c r="C32" t="n">
+        <v>2.595741987228394</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Wall Street Journal</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-0.1181042253360918</v>
+      </c>
+      <c r="C33" t="n">
+        <v>-0.3628725111484528</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-0.7780559099565219</v>
+      </c>
+      <c r="C34" t="n">
+        <v>2.213074207305908</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News**</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>-1.695816098521653</v>
+      </c>
+      <c r="C35" t="n">
+        <v>-1.473943948745728</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col width="23.83203125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="26" bestFit="1" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Linear Predicted Difference</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>XGBoost Predicted Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>pollster_CBS News</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2.546659940216689</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.507131338119507</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>pollster_CNN</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3.541705318401944</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2.67209529876709</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Daily Kos/Civiqs</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1436840326248747</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.6253640651702881</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Data for Progress (D)**</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-1.69776806930623</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-2.105467796325684</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Economist/YouGov</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.5005017311873332</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.8439670205116272</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Emerson</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2.259091309584217</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.6997199654579163</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>pollster_FOX News</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.8867105835108</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2.942646741867065</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Federalist/Susquehanna</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-1.6275697573413</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-2.342971563339233</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Grinnell/Selzer</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.6688739449781225</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.9800370335578918</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>pollster_HarrisX**</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>6.044591596331863</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2.790775775909424</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Harvard-Harris</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>5.413874847211464</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3.904946088790894</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>pollster_I&amp;I/TIPP</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1.034024870963508</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8473997116088867</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Insider Advantage</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5.540887384356907</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3.913516998291016</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>pollster_InsiderAdvantage</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.198601675865866</v>
+      </c>
+      <c r="C15" t="n">
+        <v>6.92725133895874</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Marist</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-0.01898488069880688</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.7555193901062012</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Marquette</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>3.094263617921784</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.642722368240356</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Morning Consult</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.7759223794114765</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1.005954146385193</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>pollster_NBC News</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1.43126049951471</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3.266222476959229</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>pollster_NPR/PBS/Marist</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-1.250821852173749</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-1.592438220977783</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>pollster_NY Times/Siena</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-0.5735690813159779</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-2.366077661514282</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="inlineStr">
+        <is>
+          <t>pollster_New York Post</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>3.844763019398308</v>
+      </c>
+      <c r="C22" t="n">
+        <v>3.538526296615601</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>pollster_PPP (D)</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>-2.107334466802826</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-0.7682230472564697</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Politico/Morning Consult</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.7588907442015889</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.6024054884910583</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Quinnipiac</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-1.414652883208434</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-5.46090030670166</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Rasmussen Reports</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>6.068481442200456</v>
+      </c>
+      <c r="C26" t="n">
+        <v>5.318080425262451</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Reuters/Ipsos</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2.508057137641826</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1.285426497459412</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>pollster_SurveyUSA</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.7332840285685616</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.9214429259300232</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Susquehanna</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>-11.18165379402255</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-8.744119644165039</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>pollster_The Messenger/HarrisX</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>3.988857978110061</v>
+      </c>
+      <c r="C30" t="n">
+        <v>3.60378098487854</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Trafalgar Group (R)</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>6.1346083955554</v>
+      </c>
+      <c r="C31" t="n">
+        <v>5.170015335083008</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="inlineStr">
+        <is>
+          <t>pollster_USA Today/Suffolk</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>-0.6916558018166166</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.5745726823806763</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Wall Street Journal</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-0.1106453842698851</v>
+      </c>
+      <c r="C33" t="n">
+        <v>-2.235291957855225</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-0.7710512655192598</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.2482214421033859</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News**</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>-1.686093288930358</v>
+      </c>
+      <c r="C35" t="n">
+        <v>-3.09630823135376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed The linear sine model
</commit_message>
<xml_diff>
--- a/Datasets/Predictions.xlsx
+++ b/Datasets/Predictions.xlsx
@@ -17,6 +17,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02-27-2024" sheetId="9" state="visible" r:id="rId9"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02-28-2024" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02-29-2024" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="03-01-2024" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="03-02-2024" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0009999999999999445"/>
@@ -1890,6 +1892,965 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Linear Predicted Difference</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>XGBoost Predicted Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>pollster_CBS News</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2.55735312101535</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.428045749664307</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>pollster_CNN</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3.552435299359359</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2.704452753067017</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Daily Kos/Civiqs</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1573702929926828</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.6290268301963806</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Data for Progress (D)**</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-1.685259414014917</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-2.005419492721558</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Economist/YouGov</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4935147355608027</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.002308783587068319</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Emerson</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2.266349808910419</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.6656510233879089</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>pollster_FOX News</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.896363546491922</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2.818512916564941</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Federalist/Susquehanna</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-1.623009936314896</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-2.209126472473145</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Grinnell/Selzer</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.6786593885306607</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1.1358642578125</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>pollster_HarrisX**</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>6.059013859872003</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2.914090871810913</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Harvard-Harris</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>5.420697877993796</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4.099342823028564</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>pollster_I&amp;I/TIPP</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1.045554642035351</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8425951600074768</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Insider Advantage</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5.544195999989706</v>
+      </c>
+      <c r="C14" t="n">
+        <v>4.250433444976807</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>pollster_InsiderAdvantage</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4.208166318466964</v>
+      </c>
+      <c r="C15" t="n">
+        <v>7.006680965423584</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Marist</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-0.01151784714039916</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.9264268279075623</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Marquette</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>3.100889504997216</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.376412630081177</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Morning Consult</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.7862631708123846</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1.009001135826111</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="inlineStr">
+        <is>
+          <t>pollster_NBC News</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1.440953942670495</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3.303689002990723</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>pollster_NPR/PBS/Marist</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-1.239776003188227</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-1.770082592964172</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="inlineStr">
+        <is>
+          <t>pollster_NY Times/Siena</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-0.5649538828080178</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-2.049990892410278</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="inlineStr">
+        <is>
+          <t>pollster_New York Post</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>3.85324205731877</v>
+      </c>
+      <c r="C22" t="n">
+        <v>3.715561151504517</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>pollster_PPP (D)</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>-2.106638662432982</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-1.068375587463379</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Politico/Morning Consult</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.7605801528544447</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.6613050103187561</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Quinnipiac</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-1.40710375698842</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-5.379960536956787</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Rasmussen Reports</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>6.077012849577852</v>
+      </c>
+      <c r="C26" t="n">
+        <v>5.243505954742432</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Reuters/Ipsos</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2.517180178338744</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1.322910666465759</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="7" t="inlineStr">
+        <is>
+          <t>pollster_SurveyUSA</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.7425910700587028</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1.041263937950134</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Susquehanna</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>-11.18040598727329</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-7.766969203948975</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="7" t="inlineStr">
+        <is>
+          <t>pollster_The Messenger/HarrisX</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>3.998123619421742</v>
+      </c>
+      <c r="C30" t="n">
+        <v>3.695779085159302</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Trafalgar Group (R)</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>6.140934624196198</v>
+      </c>
+      <c r="C31" t="n">
+        <v>5.420891284942627</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="7" t="inlineStr">
+        <is>
+          <t>pollster_USA Today/Suffolk</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>-0.6806780331245896</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.6375436782836914</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Wall Street Journal</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-0.102497547776732</v>
+      </c>
+      <c r="C33" t="n">
+        <v>-2.372321844100952</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-0.761712023890305</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.3949662446975708</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News**</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>-1.683884078036758</v>
+      </c>
+      <c r="C35" t="n">
+        <v>-3.230232238769531</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Linear Predicted Difference</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>XGBoost Predicted Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>pollster_CBS News</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2.596673397619933</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4.145450592041016</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>pollster_CNN</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3.591454679856594</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5.368276119232178</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Daily Kos/Civiqs</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1722176861934672</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.798820734024048</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Data for Progress (D)**</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-1.66078334537639</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1950432509183884</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Economist/YouGov</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.5466924103169304</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.431107759475708</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Emerson</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2.333753722207729</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3.038323640823364</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>pollster_FOX News</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.944189153066569</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5.414598941802979</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Federalist/Susquehanna</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-1.533540308473303</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.214027464389801</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Forbes/HarrisX</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4.020874871053748</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3.995976448059082</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Grinnell/Selzer</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.725401769118212</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3.694656133651733</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>pollster_HarrisX**</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>6.067843330924676</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4.926626205444336</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Harvard-Harris</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>5.491662395228951</v>
+      </c>
+      <c r="C13" t="n">
+        <v>6.351988315582275</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>pollster_I&amp;I/TIPP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1.078034547131181</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3.249961137771606</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Insider Advantage</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>5.643896095483688</v>
+      </c>
+      <c r="C15" t="n">
+        <v>5.89842414855957</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t>pollster_InsiderAdvantage</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4.256714075698859</v>
+      </c>
+      <c r="C16" t="n">
+        <v>9.394993782043457</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Marist</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.05418098821487671</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3.618716716766357</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Marquette</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>3.17346596566497</v>
+      </c>
+      <c r="C18" t="n">
+        <v>4.074489116668701</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Morning Consult</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.8284647555971447</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3.218261241912842</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>pollster_NBC News</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1.488448563526754</v>
+      </c>
+      <c r="C20" t="n">
+        <v>5.681851387023926</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="inlineStr">
+        <is>
+          <t>pollster_NPR/PBS/Marist</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-1.203339314279646</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1.047272682189941</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="inlineStr">
+        <is>
+          <t>pollster_NY Times/Siena</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.2462766401719474</v>
+      </c>
+      <c r="C22" t="n">
+        <v>3.998223304748535</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>pollster_New York Post</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>3.910666249720252</v>
+      </c>
+      <c r="C23" t="n">
+        <v>5.489115238189697</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="inlineStr">
+        <is>
+          <t>pollster_PPP (D)</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>-1.985574943312053</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1.7064288854599</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Politico/Morning Consult</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.8735196770749796</v>
+      </c>
+      <c r="C25" t="n">
+        <v>3.102028369903564</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Quinnipiac</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>-1.342076151411259</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-3.36479663848877</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Rasmussen Reports</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>6.134008843672303</v>
+      </c>
+      <c r="C27" t="n">
+        <v>7.477080821990967</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Reuters/Ipsos</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>2.569338688860061</v>
+      </c>
+      <c r="C28" t="n">
+        <v>3.978230237960815</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="7" t="inlineStr">
+        <is>
+          <t>pollster_SurveyUSA</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.7932451000428746</v>
+      </c>
+      <c r="C29" t="n">
+        <v>3.724176645278931</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Susquehanna</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>-11.06385570976372</v>
+      </c>
+      <c r="C30" t="n">
+        <v>-5.112802982330322</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="7" t="inlineStr">
+        <is>
+          <t>pollster_The Messenger/HarrisX</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>4.049116157526757</v>
+      </c>
+      <c r="C31" t="n">
+        <v>6.089783191680908</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Trafalgar Group (R)</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>6.215961238881561</v>
+      </c>
+      <c r="C32" t="n">
+        <v>7.117432594299316</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="7" t="inlineStr">
+        <is>
+          <t>pollster_USA Today/Suffolk</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-0.6436846864172514</v>
+      </c>
+      <c r="C33" t="n">
+        <v>3.104370832443237</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Wall Street Journal</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-0.04236529040875592</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.1708746999502182</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>-0.7113212780000966</v>
+      </c>
+      <c r="C35" t="n">
+        <v>2.56526517868042</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News**</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>-1.575194711333626</v>
+      </c>
+      <c r="C36" t="n">
+        <v>-0.825940728187561</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Improved our prediction models
</commit_message>
<xml_diff>
--- a/Datasets/Predictions.xlsx
+++ b/Datasets/Predictions.xlsx
@@ -19,6 +19,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02-29-2024" sheetId="11" state="visible" r:id="rId11"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="03-01-2024" sheetId="12" state="visible" r:id="rId12"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="03-02-2024" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="03-04-2024" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0009999999999999445"/>
@@ -2851,6 +2852,492 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>Linear Predicted Difference</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>XGBoost Predicted Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>pollster_CBS News</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2.979146416265712</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4.00047492980957</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>pollster_CNN</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3.626193239010402</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4.239157676696777</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Daily Kos/Civiqs</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.190029740162176</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.6000427603721619</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Data for Progress (D)**</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-1.63622878311821</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.5388095378875732</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Economist/YouGov</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.5913453566599141</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.2207345068454742</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Emerson</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2.388368633923411</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2.367549180984497</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>pollster_FOX News</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.993008002753223</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2.008151531219482</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Federalist/Susquehanna</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-1.463473815260776</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.3346356451511383</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Forbes/HarrisX</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4.032576526884927</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3.993991374969482</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Grinnell/Selzer</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.7655483817959134</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2.957591772079468</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>pollster_HarrisX**</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>6.08144131721248</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3.907510280609131</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Harvard-Harris</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>5.548770630322538</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5.454885959625244</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>pollster_I&amp;I/TIPP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1.108193819404871</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2.488911628723145</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Insider Advantage</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>5.721126503753778</v>
+      </c>
+      <c r="C15" t="n">
+        <v>6.177573680877686</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t>pollster_InsiderAdvantage</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4.298124908680473</v>
+      </c>
+      <c r="C16" t="n">
+        <v>8.999295234680176</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Marist</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.1076019140876214</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2.763167858123779</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Marquette</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>3.23170296888737</v>
+      </c>
+      <c r="C18" t="n">
+        <v>3.062516689300537</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Morning Consult</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.8654316626610732</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1.386166334152222</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>pollster_NBC News</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1.529121934664625</v>
+      </c>
+      <c r="C20" t="n">
+        <v>4.941399097442627</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="inlineStr">
+        <is>
+          <t>pollster_NPR/PBS/Marist</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-1.170409292505658</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-0.1794064790010452</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="inlineStr">
+        <is>
+          <t>pollster_NY Times/Siena</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.2872660663858095</v>
+      </c>
+      <c r="C22" t="n">
+        <v>3.989426374435425</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>pollster_New York Post</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>3.958292832531872</v>
+      </c>
+      <c r="C23" t="n">
+        <v>5.080272674560547</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="inlineStr">
+        <is>
+          <t>pollster_PPP (D)</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>-1.893384594774512</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1.541472673416138</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Politico/Morning Consult</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.9600210342433173</v>
+      </c>
+      <c r="C25" t="n">
+        <v>2.613255023956299</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Quinnipiac</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>-1.289125256164448</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-4.212547779083252</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Rasmussen Reports</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>6.1813355793603</v>
+      </c>
+      <c r="C27" t="n">
+        <v>6.469841003417969</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Reuters/Ipsos</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>2.613277962450671</v>
+      </c>
+      <c r="C28" t="n">
+        <v>3.117225646972656</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="7" t="inlineStr">
+        <is>
+          <t>pollster_SurveyUSA</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.8361308567132144</v>
+      </c>
+      <c r="C29" t="n">
+        <v>2.982498407363892</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Susquehanna</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>-10.97482591198693</v>
+      </c>
+      <c r="C30" t="n">
+        <v>-5.189321994781494</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="7" t="inlineStr">
+        <is>
+          <t>pollster_The Messenger/HarrisX</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>4.092238955504145</v>
+      </c>
+      <c r="C31" t="n">
+        <v>5.287618160247803</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Trafalgar Group (R)</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>6.275913969659769</v>
+      </c>
+      <c r="C32" t="n">
+        <v>6.502898693084717</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="7" t="inlineStr">
+        <is>
+          <t>pollster_USA Today/Suffolk</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-0.6103648633827659</v>
+      </c>
+      <c r="C33" t="n">
+        <v>2.252734899520874</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Wall Street Journal</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.2322041677508757</v>
+      </c>
+      <c r="C34" t="n">
+        <v>2.000150442123413</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>-0.6686198867908484</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1.965161204338074</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="7" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News**</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>-1.491669539464996</v>
+      </c>
+      <c r="C36" t="n">
+        <v>-1.131961822509766</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Completely rewrote the elections_mapping.Rmd file
</commit_message>
<xml_diff>
--- a/Datasets/Predictions.xlsx
+++ b/Datasets/Predictions.xlsx
@@ -45,6 +45,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="04-07-2024" sheetId="37" state="visible" r:id="rId37"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="04-08-2024" sheetId="38" state="visible" r:id="rId38"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="04-09-2024" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="04-11-2024" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="04-12-2024" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="04-14-2024" sheetId="42" state="visible" r:id="rId42"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0009999999999999445"/>
@@ -16708,6 +16711,1503 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>Linear Predicted Difference</t>
+        </is>
+      </c>
+      <c r="C1" s="8" t="inlineStr">
+        <is>
+          <t>XGBoost Predicted Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8" t="inlineStr">
+        <is>
+          <t>pollster_CBS News</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3.01310983210497</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2.818302869796753</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>pollster_CNBC</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.097541671051663</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.9133461117744446</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="inlineStr">
+        <is>
+          <t>pollster_CNN</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3.623182898398906</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.868304967880249</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Daily Kos/Civiqs</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-0.288659712716882</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-1.208311796188354</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Data for Progress (D)**</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-1.258177940512924</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.154130756855011</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Economist/YouGov</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.622044489757335</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.192149758338928</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Emerson</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2.051722130787175</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.074918627738953</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>pollster_FOX News</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2.42323291236444</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4.088613986968994</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Federalist/Susquehanna</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-1.695380149657371</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-2.422943353652954</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Forbes/HarrisX</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2.795367482639761</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.2919324040412903</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Grinnell/Selzer</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2.853555578953521</v>
+      </c>
+      <c r="C12" t="n">
+        <v>6.110532283782959</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8" t="inlineStr">
+        <is>
+          <t>pollster_HarrisX**</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>6.215404523576925</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2.724527597427368</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Harvard-Harris</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5.278178350867213</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3.228254795074463</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="8" t="inlineStr">
+        <is>
+          <t>pollster_I&amp;I/TIPP</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.2676307228266257</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-2.599893808364868</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Insider Advantage</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>5.442803884335579</v>
+      </c>
+      <c r="C16" t="n">
+        <v>4.016448497772217</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>pollster_InsiderAdvantage</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4.251883714371464</v>
+      </c>
+      <c r="C17" t="n">
+        <v>7.46767520904541</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Marist</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-0.01645481687616446</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.6255415081977844</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Marquette</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2.699507204163951</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1.287689566612244</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Morning Consult</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.6803109234201639</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9914634227752686</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="inlineStr">
+        <is>
+          <t>pollster_NBC News</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1.487658887341273</v>
+      </c>
+      <c r="C21" t="n">
+        <v>3.395780563354492</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="8" t="inlineStr">
+        <is>
+          <t>pollster_NPR/PBS/Marist</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-1.317168728284151</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-0.8044599294662476</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="inlineStr">
+        <is>
+          <t>pollster_NY Times/Siena</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.2437552417844273</v>
+      </c>
+      <c r="C23" t="n">
+        <v>2.22638201713562</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="8" t="inlineStr">
+        <is>
+          <t>pollster_New York Post</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>3.871778685041552</v>
+      </c>
+      <c r="C24" t="n">
+        <v>2.998229265213013</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="8" t="inlineStr">
+        <is>
+          <t>pollster_PPP (D)</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-2.26863533879683</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-1.084766030311584</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Politico/Morning Consult</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.6216302812662571</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.3364159464836121</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Quinnipiac</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>-1.518472801330066</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-2.154293298721313</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Rasmussen Reports</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>6.362992626908322</v>
+      </c>
+      <c r="C28" t="n">
+        <v>8.090641021728516</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Reuters/Ipsos</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.724144411647007</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-3.99796199798584</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="8" t="inlineStr">
+        <is>
+          <t>pollster_SurveyUSA</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.7803333684283569</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.9060943722724915</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Susquehanna</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>-11.32959888320554</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-8.169039726257324</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="8" t="inlineStr">
+        <is>
+          <t>pollster_The Messenger/HarrisX</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>4.034905634259615</v>
+      </c>
+      <c r="C32" t="n">
+        <v>4.47327184677124</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Trafalgar Group (R)</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>6.10953650823501</v>
+      </c>
+      <c r="C33" t="n">
+        <v>5.80280065536499</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="8" t="inlineStr">
+        <is>
+          <t>pollster_USA Today/Suffolk</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-0.604182959313639</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.7943722605705261</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Wall Street Journal</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.1606312100473994</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.81117182970047</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>-0.4061919050249516</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.9622617363929749</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News**</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>-1.810777056385822</v>
+      </c>
+      <c r="C37" t="n">
+        <v>-3.208897113800049</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>Linear Predicted Difference</t>
+        </is>
+      </c>
+      <c r="C1" s="8" t="inlineStr">
+        <is>
+          <t>XGBoost Predicted Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8" t="inlineStr">
+        <is>
+          <t>pollster_CBS News</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3.017174068398871</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2.818302869796753</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>pollster_CNBC</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.101605907345564</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.9133461117744446</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="inlineStr">
+        <is>
+          <t>pollster_CNN</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3.627247134692807</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.868304967880249</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Daily Kos/Civiqs</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-0.2845954764229806</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-1.208311796188354</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Data for Progress (D)**</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-1.254113704219023</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.154130756855011</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Economist/YouGov</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.6261087260512359</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.192149758338928</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Emerson</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2.055786367081076</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.074918627738953</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>pollster_FOX News</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2.427297148658341</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4.088613986968994</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Federalist/Susquehanna</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-1.69131591336347</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-2.422943353652954</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Forbes/HarrisX</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2.799431718933662</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.2919324040412903</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Grinnell/Selzer</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2.857619815247422</v>
+      </c>
+      <c r="C12" t="n">
+        <v>6.110532283782959</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8" t="inlineStr">
+        <is>
+          <t>pollster_HarrisX**</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>6.219468759870827</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2.724527597427368</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Harvard-Harris</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5.282242587161114</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3.228254795074463</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="8" t="inlineStr">
+        <is>
+          <t>pollster_I&amp;I/TIPP</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.2716949591205271</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-2.599893808364868</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Insider Advantage</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>5.44686812062948</v>
+      </c>
+      <c r="C16" t="n">
+        <v>4.016448497772217</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>pollster_InsiderAdvantage</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4.255947950665365</v>
+      </c>
+      <c r="C17" t="n">
+        <v>7.46767520904541</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Marist</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-0.01239058058226306</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.6255415081977844</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Marquette</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2.703571440457852</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1.287689566612244</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Morning Consult</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.6843751597140648</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9914634227752686</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="inlineStr">
+        <is>
+          <t>pollster_NBC News</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1.491723123635174</v>
+      </c>
+      <c r="C21" t="n">
+        <v>3.395780563354492</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="8" t="inlineStr">
+        <is>
+          <t>pollster_NPR/PBS/Marist</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-1.313104491990249</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-0.8044599294662476</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="inlineStr">
+        <is>
+          <t>pollster_NY Times/Siena</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.2478194780783287</v>
+      </c>
+      <c r="C23" t="n">
+        <v>2.22638201713562</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="8" t="inlineStr">
+        <is>
+          <t>pollster_New York Post</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>3.875842921335453</v>
+      </c>
+      <c r="C24" t="n">
+        <v>2.998229265213013</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="8" t="inlineStr">
+        <is>
+          <t>pollster_PPP (D)</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-2.264571102502929</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-1.084766030311584</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Politico/Morning Consult</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.625694517560158</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.3364159464836121</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Quinnipiac</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>-1.514408565036165</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-2.154293298721313</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Rasmussen Reports</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>6.367056863202222</v>
+      </c>
+      <c r="C28" t="n">
+        <v>8.090641021728516</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Reuters/Ipsos</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.728208647940908</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-3.99796199798584</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="8" t="inlineStr">
+        <is>
+          <t>pollster_SurveyUSA</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.7843976047222578</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.9060943722724915</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Susquehanna</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>-11.32553464691164</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-8.169039726257324</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="8" t="inlineStr">
+        <is>
+          <t>pollster_The Messenger/HarrisX</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>4.038969870553516</v>
+      </c>
+      <c r="C32" t="n">
+        <v>4.47327184677124</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Trafalgar Group (R)</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>6.11360074452891</v>
+      </c>
+      <c r="C33" t="n">
+        <v>5.80280065536499</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="8" t="inlineStr">
+        <is>
+          <t>pollster_USA Today/Suffolk</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-0.6001187230197376</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.7943722605705261</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Wall Street Journal</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.1646954463413008</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.81117182970047</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>-0.4021276687310502</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.9622617363929749</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News**</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>-1.806712820091921</v>
+      </c>
+      <c r="C37" t="n">
+        <v>-3.208897113800049</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>Linear Predicted Difference</t>
+        </is>
+      </c>
+      <c r="C1" s="8" t="inlineStr">
+        <is>
+          <t>XGBoost Predicted Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8" t="inlineStr">
+        <is>
+          <t>pollster_CBS News</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3.03078198672831</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2.179109811782837</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>pollster_CNBC</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.110879022372717</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5650177001953125</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="inlineStr">
+        <is>
+          <t>pollster_CNN</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3.642003228305663</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.314392566680908</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Daily Kos/Civiqs</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-0.2741353247967409</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-1.680352687835693</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Data for Progress (D)**</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-1.243335596359601</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.1483853906393051</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Economist/YouGov</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.6424334037455357</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.151769757270813</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Emerson</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2.073808985408894</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.6787270307540894</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>pollster_FOX News</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2.441457705201734</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3.919795036315918</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Federalist/Susquehanna</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-1.669451731528553</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-2.875464677810669</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Forbes/HarrisX</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2.809029855885826</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-0.1045597940683365</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Grinnell/Selzer</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2.871301923363468</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5.891177654266357</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8" t="inlineStr">
+        <is>
+          <t>pollster_HarrisX**</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>6.229971305661961</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2.300083160400391</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Harvard-Harris</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5.301126616258478</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2.561721086502075</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="8" t="inlineStr">
+        <is>
+          <t>pollster_I&amp;I/TIPP</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.2842324248003596</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-2.829966068267822</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Insider Advantage</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>5.470173704051695</v>
+      </c>
+      <c r="C16" t="n">
+        <v>3.48263144493103</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>pollster_InsiderAdvantage</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4.272046526150138</v>
+      </c>
+      <c r="C17" t="n">
+        <v>6.942870140075684</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Marist</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.006124462270075348</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.3486727774143219</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Marquette</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2.72173143218226</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.8213879466056824</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Morning Consult</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.6986573083109042</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.8958058953285217</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="inlineStr">
+        <is>
+          <t>pollster_NBC News</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1.507673319546248</v>
+      </c>
+      <c r="C21" t="n">
+        <v>3.008621454238892</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="8" t="inlineStr">
+        <is>
+          <t>pollster_NPR/PBS/Marist</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-1.299812410185721</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-1.27088463306427</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="inlineStr">
+        <is>
+          <t>pollster_NY Times/Siena</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.371346587604954</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1.007685661315918</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="8" t="inlineStr">
+        <is>
+          <t>pollster_New York Post</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>3.893192124668206</v>
+      </c>
+      <c r="C24" t="n">
+        <v>3.420784473419189</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="8" t="inlineStr">
+        <is>
+          <t>pollster_PPP (D)</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-2.238255533412802</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-1.373463034629822</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Politico/Morning Consult</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.6508654442146216</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-0.1043970286846161</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Quinnipiac</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>-1.496659645296796</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-2.455780506134033</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Rasmussen Reports</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>6.383271316069293</v>
+      </c>
+      <c r="C28" t="n">
+        <v>7.798167705535889</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Reuters/Ipsos</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.7422793692307494</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-4.013906955718994</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="8" t="inlineStr">
+        <is>
+          <t>pollster_SurveyUSA</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.8007929393578341</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.5623325705528259</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Susquehanna</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>-11.29985499028649</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-8.404099464416504</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="8" t="inlineStr">
+        <is>
+          <t>pollster_The Messenger/HarrisX</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>4.055412898623313</v>
+      </c>
+      <c r="C32" t="n">
+        <v>3.61281418800354</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Trafalgar Group (R)</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>6.133430006475649</v>
+      </c>
+      <c r="C33" t="n">
+        <v>5.465739250183105</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="8" t="inlineStr">
+        <is>
+          <t>pollster_USA Today/Suffolk</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-0.5856480834465385</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.1860129237174988</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Wall Street Journal</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.1815806690974995</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.3445440232753754</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>-0.3865189813674128</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.5874801874160767</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News**</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>-1.782140711008176</v>
+      </c>
+      <c r="C37" t="n">
+        <v>-3.604949235916138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Removed a not needed file
</commit_message>
<xml_diff>
--- a/Datasets/Predictions.xlsx
+++ b/Datasets/Predictions.xlsx
@@ -50,6 +50,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="04-14-2024" sheetId="42" state="visible" r:id="rId42"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="04-16-2024" sheetId="43" state="visible" r:id="rId43"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="04-19-2024" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="04-21-2024" sheetId="45" state="visible" r:id="rId45"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0009999999999999445"/>
@@ -19208,6 +19209,505 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>Linear Predicted Difference</t>
+        </is>
+      </c>
+      <c r="C1" s="8" t="inlineStr">
+        <is>
+          <t>XGBoost Predicted Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8" t="inlineStr">
+        <is>
+          <t>pollster_CBS News</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3.072917012648367</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2.549972295761108</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>pollster_CNBC</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.142966447193374</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.8700668811798096</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="inlineStr">
+        <is>
+          <t>pollster_CNN</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3.686799599260403</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.971726894378662</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Daily Kos/Civiqs</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.182212138579338</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.9383037686347961</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Data for Progress (D)**</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-1.207759762355517</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.3364807069301605</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Economist/YouGov</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.6908655814551774</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.7516812086105347</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Emerson</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2.159319310666717</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2.989696025848389</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>pollster_FOX News</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2.484873686204431</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4.331109046936035</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Federalist/Susquehanna</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-1.608179587621299</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-2.487954378128052</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Forbes/HarrisX</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2.841870646069874</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.3763706684112549</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Grinnell/Selzer</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2.913608913116613</v>
+      </c>
+      <c r="C12" t="n">
+        <v>6.060928344726562</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8" t="inlineStr">
+        <is>
+          <t>pollster_HarrisX**</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>6.264908416857561</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2.607294082641602</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Harvard-Harris</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5.355491091275961</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2.15910530090332</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="8" t="inlineStr">
+        <is>
+          <t>pollster_I&amp;I/TIPP</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.3238862582728297</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-2.186527252197266</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Insider Advantage</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>5.534786859571602</v>
+      </c>
+      <c r="C16" t="n">
+        <v>4.231391429901123</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>pollster_InsiderAdvantage</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4.319954623606749</v>
+      </c>
+      <c r="C17" t="n">
+        <v>7.111198425292969</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Marist</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.05963366743036502</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.717138946056366</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Marquette</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2.774417667570467</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.8810979127883911</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Morning Consult</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.7243218602052033</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.01597485318779945</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="inlineStr">
+        <is>
+          <t>pollster_NBC News</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1.649235866076296</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1.948659896850586</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="8" t="inlineStr">
+        <is>
+          <t>pollster_NPR/PBS/Marist</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-1.258409458868962</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-1.311262249946594</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="inlineStr">
+        <is>
+          <t>pollster_NY Times/Siena</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.4165032637335209</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1.131097793579102</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="8" t="inlineStr">
+        <is>
+          <t>pollster_New York Post</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>3.943999041024175</v>
+      </c>
+      <c r="C24" t="n">
+        <v>3.40349555015564</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="8" t="inlineStr">
+        <is>
+          <t>pollster_PPP (D)</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-2.166665559525594</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-1.257511377334595</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Politico/Morning Consult</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.7198022618213797</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.2121571153402328</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Quinnipiac</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>-1.444926229922307</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-2.618772268295288</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Rasmussen Reports</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>6.431448004655588</v>
+      </c>
+      <c r="C28" t="n">
+        <v>7.59668493270874</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Reuters/Ipsos</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.7854871219188557</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-3.087626457214355</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="8" t="inlineStr">
+        <is>
+          <t>pollster_SurveyUSA</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.8493888921466355</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.8449379205703735</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Susquehanna</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>-11.22973899211079</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-7.595902919769287</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="8" t="inlineStr">
+        <is>
+          <t>pollster_The Messenger/HarrisX</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>4.104119399590374</v>
+      </c>
+      <c r="C32" t="n">
+        <v>4.241454601287842</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Trafalgar Group (R)</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>6.189985428106216</v>
+      </c>
+      <c r="C33" t="n">
+        <v>5.265925884246826</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="8" t="inlineStr">
+        <is>
+          <t>pollster_USA Today/Suffolk</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-0.5415133638111804</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.6435413956642151</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Wall Street Journal</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.2313121291008491</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.6309971809387207</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>-0.302828325158921</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.1194566562771797</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="8" t="inlineStr">
+        <is>
+          <t>pollster_Yahoo News**</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>-1.714591887196505</v>
+      </c>
+      <c r="C37" t="n">
+        <v>-3.566738605499268</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>